<commit_message>
(JMT) Verified dates, names, etc.
</commit_message>
<xml_diff>
--- a/blocks/bl_1s7/bl_1s7.xlsx
+++ b/blocks/bl_1s7/bl_1s7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\bl_1s7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51639E25-D4AA-4246-81E2-43B5F9466294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98756535-E964-47DF-A6A9-ECAFCD4AD40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bl_1s6" sheetId="1" r:id="rId1"/>
@@ -923,7 +923,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>